<commit_message>
Correcciones de seba de la maqueta
</commit_message>
<xml_diff>
--- a/PS hito 1 segunda correccion/Mapa de actividades prototipado Dario v1.0.xlsx
+++ b/PS hito 1 segunda correccion/Mapa de actividades prototipado Dario v1.0.xlsx
@@ -694,7 +694,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="J43" sqref="J43:K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="e">
         <f>C1:I1</f>
         <v>#VALUE!</v>

</xml_diff>